<commit_message>
All files passing and sheets_to_dataframe() now recognizes sheets adhereing to any pattern in the patterns directory. all tests passing
</commit_message>
<xml_diff>
--- a/test_graph_analysis/data_test/Composition Example.xlsx
+++ b/test_graph_analysis/data_test/Composition Example.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnelly7-gtri\Documents\Ingrid_Nerdman\test_graph_analysis\data_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="composition" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>